<commit_message>
XLS Forms Updated for 2017 First Round
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/deathtohoh.xlsx
+++ b/xforms/xlsforms/deathtohoh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13004" tabRatio="500"/>
+    <workbookView windowWidth="28695" windowHeight="12870" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,30 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>paul</author>
+  </authors>
+  <commentList>
+    <comment ref="A25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">paul:
+This field is not on database yet, I should add this variable to the ODK and see if it works</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>paul</author>
@@ -54,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216">
   <si>
     <t>type</t>
   </si>
@@ -321,6 +345,9 @@
   </si>
   <si>
     <t>processedByMirth</t>
+  </si>
+  <si>
+    <t>processedBySync</t>
   </si>
   <si>
     <t>list_name</t>
@@ -706,8 +733,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -776,8 +803,114 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,22 +925,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,102 +938,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -964,7 +991,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,13 +1105,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,157 +1165,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1207,6 +1234,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1218,21 +1263,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1252,29 +1282,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1304,155 +1322,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1586,6 +1613,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1615,6 +1645,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2002,269 +2035,269 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="$A17:$XFD20"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="11.85"/>
   <cols>
-    <col min="1" max="1" width="30.1266666666667" style="51" customWidth="1"/>
-    <col min="2" max="2" width="26.6266666666667" style="51" customWidth="1"/>
-    <col min="3" max="4" width="46.1" style="51" customWidth="1"/>
-    <col min="5" max="5" width="30.1266666666667" style="51" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="51" customWidth="1"/>
-    <col min="7" max="7" width="22.8733333333333" style="51" customWidth="1"/>
-    <col min="8" max="8" width="25" style="51" customWidth="1"/>
-    <col min="9" max="9" width="10.8733333333333" style="51"/>
-    <col min="10" max="10" width="37.2533333333333" style="51" customWidth="1"/>
-    <col min="11" max="11" width="10.8733333333333" style="51"/>
-    <col min="12" max="12" width="19.1266666666667" style="51" customWidth="1"/>
-    <col min="13" max="13" width="10.8733333333333" style="51"/>
-    <col min="14" max="14" width="13.1" style="51" customWidth="1"/>
-    <col min="15" max="17" width="10.8733333333333" style="51"/>
-    <col min="18" max="18" width="12" style="51" customWidth="1"/>
-    <col min="19" max="16384" width="10.8733333333333" style="51"/>
+    <col min="1" max="1" width="30.1266666666667" style="52" customWidth="1"/>
+    <col min="2" max="2" width="26.6266666666667" style="52" customWidth="1"/>
+    <col min="3" max="4" width="46.1" style="52" customWidth="1"/>
+    <col min="5" max="5" width="30.1266666666667" style="52" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="52" customWidth="1"/>
+    <col min="7" max="7" width="22.8733333333333" style="52" customWidth="1"/>
+    <col min="8" max="8" width="25" style="52" customWidth="1"/>
+    <col min="9" max="9" width="10.8733333333333" style="52"/>
+    <col min="10" max="10" width="37.2533333333333" style="52" customWidth="1"/>
+    <col min="11" max="11" width="10.8733333333333" style="52"/>
+    <col min="12" max="12" width="19.1266666666667" style="52" customWidth="1"/>
+    <col min="13" max="13" width="10.8733333333333" style="52"/>
+    <col min="14" max="14" width="13.1" style="52" customWidth="1"/>
+    <col min="15" max="17" width="10.8733333333333" style="52"/>
+    <col min="18" max="18" width="12" style="52" customWidth="1"/>
+    <col min="19" max="16384" width="10.8733333333333" style="52"/>
   </cols>
   <sheetData>
     <row r="1" ht="12" spans="1:18">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="P1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="52" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" ht="12" spans="1:15">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="51" t="b">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="52" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
     </row>
     <row r="3" ht="12" spans="1:15">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="51" t="b">
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="52" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
     </row>
     <row r="4" ht="12" spans="1:15">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="51" t="b">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="52" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:13">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="52" t="b">
+      <c r="I5" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="51" t="b">
+      <c r="M5" s="52" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="12" spans="1:13">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="52" t="b">
+      <c r="I6" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="M6" s="51" t="b">
+      <c r="M6" s="52" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" ht="12" spans="1:13">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="52" t="b">
+      <c r="I7" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="M7" s="51" t="b">
+      <c r="M7" s="52" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1" spans="1:13">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="52" t="b">
+      <c r="I8" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="M8" s="52" t="b">
+      <c r="M8" s="53" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1" spans="1:13">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="52" t="b">
+      <c r="I9" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="M9" s="51" t="b">
+      <c r="M9" s="52" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1" spans="1:13">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="52"/>
-      <c r="M10" s="52" t="b">
+      <c r="I10" s="53"/>
+      <c r="M10" s="53" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2281,10 +2314,10 @@
       <c r="E11" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="62" t="s">
         <v>44</v>
       </c>
       <c r="I11" s="47" t="b">
@@ -2369,19 +2402,19 @@
       </c>
     </row>
     <row r="16" s="49" customFormat="1" ht="18" customHeight="1" spans="1:11">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="K16" s="54" t="b">
+      <c r="D16" s="57"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="K16" s="55" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2398,7 +2431,7 @@
       <c r="E17" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="62" t="b">
+      <c r="I17" s="63" t="b">
         <v>1</v>
       </c>
       <c r="M17" s="50" t="b">
@@ -2423,17 +2456,17 @@
       </c>
     </row>
     <row r="19" s="50" customFormat="1" ht="12" spans="1:13">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="59" t="s">
         <v>76</v>
       </c>
       <c r="I19" s="50" t="b">
@@ -2447,14 +2480,14 @@
       <c r="A20" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58" t="s">
+      <c r="D20" s="59"/>
+      <c r="E20" s="59" t="s">
         <v>79</v>
       </c>
       <c r="I20" s="50" t="b">
@@ -2465,17 +2498,17 @@
       </c>
     </row>
     <row r="21" s="50" customFormat="1" ht="12" spans="1:13">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58" t="s">
+      <c r="D21" s="59"/>
+      <c r="E21" s="59" t="s">
         <v>82</v>
       </c>
       <c r="I21" s="50" t="b">
@@ -2508,77 +2541,87 @@
       </c>
     </row>
     <row r="24" ht="12" spans="1:13">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="51" t="s">
+      <c r="E24" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="M24" s="51" t="b">
+      <c r="M24" s="52" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:9">
-      <c r="I25" s="59"/>
+    <row r="25" s="51" customFormat="1" ht="12" spans="1:9">
+      <c r="A25" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="64"/>
     </row>
     <row r="33" spans="9:9">
-      <c r="I33" s="59"/>
+      <c r="I33" s="60"/>
     </row>
     <row r="34" spans="9:9">
-      <c r="I34" s="59"/>
+      <c r="I34" s="60"/>
     </row>
     <row r="35" spans="9:9">
-      <c r="I35" s="59"/>
+      <c r="I35" s="60"/>
     </row>
     <row r="36" spans="9:9">
-      <c r="I36" s="59"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="9:9">
-      <c r="I37" s="59"/>
+      <c r="I37" s="60"/>
     </row>
     <row r="54" spans="9:9">
-      <c r="I54" s="59"/>
+      <c r="I54" s="60"/>
     </row>
     <row r="55" spans="9:9">
-      <c r="I55" s="59"/>
+      <c r="I55" s="60"/>
     </row>
     <row r="56" spans="9:9">
-      <c r="I56" s="59"/>
+      <c r="I56" s="60"/>
     </row>
     <row r="57" spans="9:9">
-      <c r="I57" s="59"/>
+      <c r="I57" s="60"/>
     </row>
     <row r="58" spans="9:9">
-      <c r="I58" s="59"/>
+      <c r="I58" s="60"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="59"/>
-      <c r="I59" s="59"/>
+      <c r="A59" s="60"/>
+      <c r="I59" s="60"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="59"/>
-      <c r="I60" s="59"/>
+      <c r="A60" s="60"/>
+      <c r="I60" s="60"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="59"/>
-      <c r="I61" s="59"/>
+      <c r="A61" s="60"/>
+      <c r="I61" s="60"/>
     </row>
     <row r="62" spans="9:9">
-      <c r="I62" s="59"/>
+      <c r="I62" s="60"/>
     </row>
     <row r="64" spans="9:9">
-      <c r="I64" s="59"/>
+      <c r="I64" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2603,7 +2646,7 @@
   <sheetData>
     <row r="1" ht="13.5" spans="1:5">
       <c r="A1" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
@@ -2612,7 +2655,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>4</v>
@@ -2626,13 +2669,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:5">
@@ -2643,13 +2686,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" ht="18" customHeight="1" spans="1:5">
@@ -2660,13 +2703,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="1:5">
@@ -2677,13 +2720,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:5">
@@ -2694,13 +2737,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:5">
@@ -2711,13 +2754,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" spans="1:5">
@@ -2728,13 +2771,13 @@
         <v>98</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:5">
@@ -2745,336 +2788,336 @@
         <v>88</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" ht="14.1" spans="1:5">
       <c r="A10" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" ht="14.1" spans="1:5">
       <c r="A11" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" ht="14.1" spans="1:5">
       <c r="A12" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B12" s="17">
         <v>1</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" ht="14.1" spans="1:5">
       <c r="A13" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="17">
         <v>2</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1" ht="14.1" spans="1:5">
       <c r="A14" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B14" s="17">
         <v>3</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" ht="14.1" spans="1:5">
       <c r="A15" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B15" s="17">
         <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A16" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A17" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A18" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C18" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>135</v>
-      </c>
       <c r="E18" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A19" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A20" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>140</v>
-      </c>
       <c r="E20" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A21" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A22" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>143</v>
-      </c>
       <c r="E22" s="20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A23" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A24" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C24" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>146</v>
-      </c>
       <c r="E24" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A25" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A26" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C26" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>140</v>
-      </c>
       <c r="E26" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A27" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" s="4" customFormat="1" ht="14.1" spans="1:5">
       <c r="A28" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3085,13 +3128,13 @@
         <v>1</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3102,13 +3145,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D30" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="23" t="s">
         <v>156</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="31" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3119,13 +3162,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3136,13 +3179,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" s="6" customFormat="1" ht="14.1" spans="1:5">
@@ -3153,13 +3196,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" s="6" customFormat="1" ht="14.1" spans="1:5">
@@ -3170,13 +3213,13 @@
         <v>6</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3187,13 +3230,13 @@
         <v>7</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3204,13 +3247,13 @@
         <v>98</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" s="5" customFormat="1" ht="13.5" spans="1:5">
@@ -3221,574 +3264,574 @@
         <v>88</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="23"/>
     </row>
     <row r="38" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A38" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B38" s="16">
         <v>1</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B39" s="16">
         <v>2</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B40" s="16">
         <v>3</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B41" s="16">
         <v>4</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" s="8" customFormat="1" ht="14.1" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B42" s="16">
         <v>5</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B43" s="16">
         <v>6</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B44" s="16">
         <v>88</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" s="7" customFormat="1" ht="14.85" spans="1:5">
       <c r="A45" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B45" s="16">
         <v>99</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" s="9" customFormat="1" ht="14.1" spans="1:5">
       <c r="A46" s="26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B46" s="27">
         <v>1</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A47" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B47" s="16">
         <v>2</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A48" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B48" s="16">
         <v>3</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A49" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B49" s="16">
         <v>4</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A50" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B50" s="16">
         <v>5</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A51" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B51" s="16">
         <v>6</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A52" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B52" s="16">
         <v>7</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A53" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B53" s="16">
         <v>8</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B54" s="30">
         <v>9</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" s="7" customFormat="1" ht="14.1" spans="1:5">
       <c r="A55" s="29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B55" s="16">
         <v>98</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" s="10" customFormat="1" ht="14.85" spans="1:5">
       <c r="A56" s="32" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B56" s="33">
         <v>88</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E56" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B57" s="36">
         <v>1</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B58" s="36">
         <v>2</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B59" s="39">
         <v>3</v>
       </c>
       <c r="C59" s="40" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B60" s="39">
         <v>4</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B61" s="41">
         <v>5</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B62" s="41">
         <v>6</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B63" s="41">
         <v>7</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B64" s="41">
         <v>8</v>
       </c>
       <c r="C64" s="42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B65" s="41">
         <v>9</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B66" s="41">
         <v>10</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B67" s="41">
         <v>11</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B68" s="41">
         <v>12</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B69" s="41">
         <v>13</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B70" s="41">
         <v>14</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B71" s="41">
         <v>15</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B72" s="41">
         <v>16</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B73" s="41">
         <v>17</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B74" s="41">
         <v>18</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B75" s="41">
         <v>19</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B76" s="43" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B77" s="41">
         <v>88</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" ht="14.1" spans="1:3">
       <c r="A78" s="44" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B78" s="45">
         <v>99</v>
       </c>
       <c r="C78" s="46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3818,30 +3861,30 @@
   <sheetData>
     <row r="1" ht="14.25" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" ht="21" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>